<commit_message>
Update BOM,PCB for correct reference name
</commit_message>
<xml_diff>
--- a/hardware/LamdaShifter_2_0SMT_BOM - Copy.xlsx
+++ b/hardware/LamdaShifter_2_0SMT_BOM - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\PlatformIO\Projects\Lambda Shifter OTA\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3ACE6D-96C0-4583-997B-5581463641E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004CD5C2-32ED-4325-9675-8AAB2AE34E70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>Item #</t>
   </si>
@@ -257,10 +257,6 @@
   </si>
   <si>
     <t>Q2,Q3</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
-    <t>D4</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -823,7 +819,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -842,7 +838,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6"/>
       <c r="D1" s="7"/>
@@ -939,13 +935,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="G5" s="10">
         <v>2012</v>
@@ -954,7 +950,7 @@
         <v>10</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1039,28 +1035,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>